<commit_message>
I am making short description and description nullable.
I am making short description and description nullable instead of adding
a not null constraint.
</commit_message>
<xml_diff>
--- a/virtualization-software-instance.xlsx
+++ b/virtualization-software-instance.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\git\virtual-machine-database\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4102419-F5E3-4462-A2E2-0D3ACD332140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,47 +25,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t xml:space="preserve">virtualization_software_string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vmware Workstation Pro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VMware® Workstation 17 Pro 17.6.0 build-24238078</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>virtualization_software_string</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>Vmware Workstation Pro</t>
+  </si>
+  <si>
+    <t>VMware® Workstation 17 Pro 17.6.0 build-24238078</t>
+  </si>
+  <si>
+    <t>VirtualBox</t>
+  </si>
+  <si>
+    <t>Version 7.1.2 r164945 (Qt6.5.3)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,7 +65,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -80,99 +73,79 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18a303"/>
+        <a:srgbClr val="18A303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369a3"/>
+        <a:srgbClr val="0369A3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a33e03"/>
+        <a:srgbClr val="A33E03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8e03a3"/>
+        <a:srgbClr val="8E03A3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="c99c00"/>
+        <a:srgbClr val="C99C00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="c9211e"/>
+        <a:srgbClr val="C9211E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ee"/>
+        <a:srgbClr val="0000EE"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551a8b"/>
+        <a:srgbClr val="551A8B"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -225,46 +198,52 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.94"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>